<commit_message>
Changes to Data Loaders (to be tested)
</commit_message>
<xml_diff>
--- a/src/main/resources/dataloader.xlsx
+++ b/src/main/resources/dataloader.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
     <sheet name="paths" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -680,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28:C30"/>
     </sheetView>
   </sheetViews>
@@ -1028,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C6"/>
     </sheetView>
   </sheetViews>
@@ -1103,16 +1102,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>